<commit_message>
atomized OSA uca block. Created tier feature selections.
</commit_message>
<xml_diff>
--- a/ucoa.xlsx
+++ b/ucoa.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="funds full" sheetId="8" r:id="rId1"/>
@@ -4655,7 +4655,7 @@
   <dimension ref="A1:X221"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10615,8 +10615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13400,8 +13400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU335"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C285" sqref="C285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>